<commit_message>
Closes #121 - finished work on input helpers and validators for Russian identity documents
</commit_message>
<xml_diff>
--- a/DatabaseUpdate/ExcelFiles/IdentityDocumentTypes.xlsx
+++ b/DatabaseUpdate/ExcelFiles/IdentityDocumentTypes.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="IdentityDocumentTypes Data" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Data" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <x:si>
     <x:t>Id</x:t>
   </x:si>
@@ -22,28 +22,49 @@
     <x:t>Name</x:t>
   </x:si>
   <x:si>
+    <x:t>Options</x:t>
+  </x:si>
+  <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
     <x:t>Свидетельство о рождении РФ</x:t>
   </x:si>
   <x:si>
+    <x:t>IsRussianBirthCertificate</x:t>
+  </x:si>
+  <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
     <x:t>Паспорт гражданина РФ</x:t>
   </x:si>
   <x:si>
+    <x:t>IsRussianPassport</x:t>
+  </x:si>
+  <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
     <x:t>Паспорт иностранного гражданина</x:t>
   </x:si>
   <x:si>
+    <x:t>NULL</x:t>
+  </x:si>
+  <x:si>
     <x:t>4</x:t>
   </x:si>
   <x:si>
     <x:t>Удостоверение личности</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Заграничный паспорт гражданина РФ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IsRussianForeignPassport</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -394,50 +415,76 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B5"/>
+  <x:dimension ref="A1:C6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2">
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:2">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:2">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:2">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>